<commit_message>
working on state machine
</commit_message>
<xml_diff>
--- a/LAB#1/lab1_template_de1soc/lab1_ factor_divider.xlsx
+++ b/LAB#1/lab1_template_de1soc/lab1_ factor_divider.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melika\Documents\GitHub\CPEN311\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melika\Documents\GitHub\CPEN311\LAB#1\lab1_template_de1soc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D3B156-B87C-454D-B9E2-4D12BD82E096}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7376EC9-5BF4-498B-9301-FC73EE2AFAC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{EE641918-0FE9-42AB-912D-D77D9B10E8DA}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t xml:space="preserve">in </t>
   </si>
@@ -425,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50285A71-9FE1-4F97-9E33-0A3436988C65}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A13" sqref="A13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,6 +612,29 @@
         <v>25000000</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>50000000</v>
+      </c>
+      <c r="B14">
+        <v>22000</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" ref="C14" si="2">A14/(B14*2)</f>
+        <v>1136.3636363636363</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update no significant change
</commit_message>
<xml_diff>
--- a/LAB#1/lab1_template_de1soc/lab1_ factor_divider.xlsx
+++ b/LAB#1/lab1_template_de1soc/lab1_ factor_divider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melika\Documents\GitHub\CPEN311\LAB#1\lab1_template_de1soc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7376EC9-5BF4-498B-9301-FC73EE2AFAC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3764E5D3-2CE3-4329-832E-95789EBEA885}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{EE641918-0FE9-42AB-912D-D77D9B10E8DA}"/>
   </bookViews>
@@ -424,14 +424,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50285A71-9FE1-4F97-9E33-0A3436988C65}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:C14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -635,6 +637,46 @@
         <v>1136.3636363636363</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>1/A14</f>
+        <v>2E-8</v>
+      </c>
+      <c r="B16">
+        <f>1/B14</f>
+        <v>4.5454545454545452E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>A16*100000</f>
+        <v>2E-3</v>
+      </c>
+      <c r="B17">
+        <f>B16*100000</f>
+        <v>4.545454545454545</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>A17*1000</f>
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <f>B17*1000</f>
+        <v>4545.454545454545</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>A18/2</f>
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <f>B18/2</f>
+        <v>2272.7272727272725</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>